<commit_message>
stable build for overall map but changing geo file info
</commit_message>
<xml_diff>
--- a/ccc_nyc_shiny/data/nyc_geo/nyc2010census_tabulation_equiv.xlsx
+++ b/ccc_nyc_shiny/data/nyc_geo/nyc2010census_tabulation_equiv.xlsx
@@ -5,16 +5,17 @@
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de6cb9e11468ad32/Documents/Jason/NYC Data Science Academy/projects/capstone/git_work_area/ccc_nyc_shiny/data/nyc_geo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F558B8-8053-4906-92DF-160DE42C51AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{54F558B8-8053-4906-92DF-160DE42C51AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D4070F45-2C81-4A3C-83F8-91E48B3B09A3}"/>
   <bookViews>
-    <workbookView xWindow="-21765" yWindow="-21030" windowWidth="25605" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28875" yWindow="-21600" windowWidth="25590" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NTA to 2010 CT equivalency" sheetId="2" r:id="rId1"/>
     <sheet name="NTA in PUMA_" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'NTA in PUMA_'!$F$1:$F$226</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16730" uniqueCount="1866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16748" uniqueCount="1866">
   <si>
     <t>Borough</t>
   </si>
@@ -5776,7 +5777,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -5827,6 +5828,9 @@
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6169,7 +6173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -56135,8 +56139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H226"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A170" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -61291,4 +61295,88 @@
     <oddFooter>&amp;L&amp;"Arial,Regular"&amp;9Population Division - NYC Department of City Planning (August 2012)&amp;R&amp;"Arial,Regular"&amp;9&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7811D5A5-392F-4C44-A206-F44FC96ABF5C}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C6">
+    <sortCondition ref="C2:C6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>